<commit_message>
Updating Bulk table guide and example input with new variable names
</commit_message>
<xml_diff>
--- a/www/example-NPM-data.xlsx
+++ b/www/example-NPM-data.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25601"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28025"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://leeds365-my.sharepoint.com/personal/medacola_leeds_ac_uk/Documents/RC/Projects/rse-projects/2023-04-nutrientprofiler/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\maeve\Documents\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="54" documentId="8_{6402FB9C-BD51-496C-8DBC-3FDD79349D50}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{96D20204-8F11-42F1-8122-468F9EE5C995}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{E63A4015-A377-4DAC-B30C-D526C7ED5D35}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="npm-testcases" sheetId="1" r:id="rId1"/>
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="46" uniqueCount="43">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="61" uniqueCount="57">
   <si>
     <t>name</t>
   </si>
@@ -56,9 +56,6 @@
     <t>sugar_measurement_g</t>
   </si>
   <si>
-    <t>fat_measurement_g</t>
-  </si>
-  <si>
     <t>salt_measurement_g</t>
   </si>
   <si>
@@ -74,9 +71,6 @@
     <t>protein_measurement_g</t>
   </si>
   <si>
-    <t>fruit_nut_measurement_percent</t>
-  </si>
-  <si>
     <t>weight_g</t>
   </si>
   <si>
@@ -150,6 +144,54 @@
   </si>
   <si>
     <t>Whipping cream</t>
+  </si>
+  <si>
+    <t>satfat_measurement_g</t>
+  </si>
+  <si>
+    <t>fvn_measurement_percent</t>
+  </si>
+  <si>
+    <t>Soft drink</t>
+  </si>
+  <si>
+    <t>Savory snack</t>
+  </si>
+  <si>
+    <t>Breakfast cereals</t>
+  </si>
+  <si>
+    <t>Confectionary</t>
+  </si>
+  <si>
+    <t>Ices</t>
+  </si>
+  <si>
+    <t>Cakes</t>
+  </si>
+  <si>
+    <t>Sweet biscuits and bars</t>
+  </si>
+  <si>
+    <t>Morning goods</t>
+  </si>
+  <si>
+    <t>Desserts and puddings</t>
+  </si>
+  <si>
+    <t>Yoghurts</t>
+  </si>
+  <si>
+    <t>Pizza</t>
+  </si>
+  <si>
+    <t>Potato products</t>
+  </si>
+  <si>
+    <t>Ready meals and meal centres</t>
+  </si>
+  <si>
+    <t>Other</t>
   </si>
 </sst>
 </file>
@@ -694,10 +736,14 @@
 </styleSheet>
 </file>
 
+<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
+<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
+</file>
+
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office 2013 - 2022 Theme">
   <a:themeElements>
-    <a:clrScheme name="Office">
+    <a:clrScheme name="Office 2013 - 2022">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -735,7 +781,7 @@
         <a:srgbClr val="954F72"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office">
+    <a:fontScheme name="Office 2013 - 2022">
       <a:majorFont>
         <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
@@ -841,7 +887,7 @@
         <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office">
+    <a:fmtScheme name="Office 2013 - 2022">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -983,7 +1029,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office 2013 - 2022 Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -993,34 +1039,34 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:U1"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G11" sqref="G11"/>
+    <sheetView tabSelected="1" topLeftCell="H1" workbookViewId="0">
+      <selection activeCell="S2" sqref="S2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="3" max="3" width="15.5546875" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="11.88671875" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="9.44140625" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="11.6640625" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="19.77734375" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="25.5546875" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="21.33203125" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="23.21875" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="19.6640625" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="17.6640625" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="18.21875" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="22.88671875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="15.5703125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="11.85546875" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="9.42578125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="11.7109375" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="19.7109375" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="25.5703125" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="21.28515625" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="23.28515625" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="19.7109375" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="17.7109375" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="18.28515625" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="22.85546875" bestFit="1" customWidth="1"/>
     <col min="15" max="15" width="21" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="22.33203125" bestFit="1" customWidth="1"/>
-    <col min="17" max="17" width="21.33203125" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="22.28515625" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="21.28515625" bestFit="1" customWidth="1"/>
     <col min="18" max="18" width="28" bestFit="1" customWidth="1"/>
-    <col min="19" max="19" width="8.44140625" customWidth="1"/>
+    <col min="19" max="19" width="8.42578125" customWidth="1"/>
     <col min="20" max="20" width="10" bestFit="1" customWidth="1"/>
-    <col min="21" max="21" width="15.88671875" bestFit="1" customWidth="1"/>
+    <col min="21" max="21" width="15.85546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:21" s="1" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:21" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -1055,34 +1101,34 @@
         <v>10</v>
       </c>
       <c r="L1" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="M1" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="M1" s="1" t="s">
+      <c r="N1" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="N1" s="1" t="s">
+      <c r="O1" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="O1" s="1" t="s">
+      <c r="P1" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="P1" s="1" t="s">
+      <c r="Q1" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="Q1" s="1" t="s">
+      <c r="R1" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="S1" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="R1" s="1" t="s">
+      <c r="T1" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="S1" s="1" t="s">
+      <c r="U1" s="1" t="s">
         <v>18</v>
-      </c>
-      <c r="T1" s="1" t="s">
-        <v>19</v>
-      </c>
-      <c r="U1" s="1" t="s">
-        <v>20</v>
       </c>
     </row>
   </sheetData>
@@ -1090,30 +1136,36 @@
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="0" copies="0" r:id="rId1"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{CCE6A557-97BC-4b89-ADB6-D9C93CAAB3DF}">
-      <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="4">
+      <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="5">
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{EBCE890A-C11A-4240-8C99-DDC1B2D3DE56}">
           <x14:formula1>
-            <xm:f>validation!$A$2:$A$3</xm:f>
+            <xm:f>validation!$B$2:$B$3</xm:f>
           </x14:formula1>
           <xm:sqref>D2:D257</xm:sqref>
         </x14:dataValidation>
         <x14:dataValidation type="list" showInputMessage="1" showErrorMessage="1" xr:uid="{F16BA462-123E-40A6-9FDF-BACDD6071EA4}">
           <x14:formula1>
-            <xm:f>validation!$C$2:$C$5</xm:f>
+            <xm:f>validation!$D$2:$D$5</xm:f>
           </x14:formula1>
           <xm:sqref>F2:F203</xm:sqref>
         </x14:dataValidation>
         <x14:dataValidation type="list" showInputMessage="1" showErrorMessage="1" xr:uid="{7419570C-CAF2-4CF8-88A6-DE0CAFBC2EF9}">
           <x14:formula1>
-            <xm:f>validation!$B$2:$B$15</xm:f>
+            <xm:f>validation!$C$2:$C$15</xm:f>
           </x14:formula1>
           <xm:sqref>E2:E302 G2:G343</xm:sqref>
         </x14:dataValidation>
         <x14:dataValidation type="list" showInputMessage="1" showErrorMessage="1" xr:uid="{F1F9E6F3-CDED-4F25-9DBC-4A3901DAA168}">
           <x14:formula1>
-            <xm:f>validation!$D$2:$D$5</xm:f>
+            <xm:f>validation!$E$2:$E$5</xm:f>
           </x14:formula1>
           <xm:sqref>H2:H299</xm:sqref>
+        </x14:dataValidation>
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{AF59734F-CAFE-44DE-A859-6BEF3351FA1E}">
+          <x14:formula1>
+            <xm:f>validation!$A$2:$A$15</xm:f>
+          </x14:formula1>
+          <xm:sqref>C2:C1048576</xm:sqref>
         </x14:dataValidation>
       </x14:dataValidations>
     </ext>
@@ -1123,124 +1175,471 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EA1956F8-7C50-4F3B-9EB1-0BC845BC0782}">
-  <dimension ref="A1:D14"/>
+  <dimension ref="A1:E15"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B15" sqref="B15"/>
+      <selection activeCell="C1" sqref="C1:C1048576"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="12.6640625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="9.44140625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="11.6640625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="28.77734375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="12.7109375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="9.42578125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="11.7109375" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="28.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
+        <v>2</v>
+      </c>
+      <c r="B1" t="s">
+        <v>28</v>
+      </c>
+      <c r="C1" t="s">
+        <v>4</v>
+      </c>
+      <c r="D1" t="s">
+        <v>5</v>
+      </c>
+      <c r="E1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>43</v>
+      </c>
+      <c r="B2" t="s">
+        <v>19</v>
+      </c>
+      <c r="C2" t="s">
         <v>30</v>
       </c>
-      <c r="B1" t="s">
-        <v>4</v>
-      </c>
-      <c r="C1" t="s">
-        <v>5</v>
-      </c>
-      <c r="D1" t="s">
-        <v>7</v>
+      <c r="D2" t="s">
+        <v>22</v>
+      </c>
+      <c r="E2" t="s">
+        <v>25</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A2" t="s">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>44</v>
+      </c>
+      <c r="B3" t="s">
         <v>21</v>
       </c>
-      <c r="B2" t="s">
+      <c r="C3" t="s">
+        <v>23</v>
+      </c>
+      <c r="D3" t="s">
+        <v>26</v>
+      </c>
+      <c r="E3" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>45</v>
+      </c>
+      <c r="C4" t="s">
+        <v>31</v>
+      </c>
+      <c r="D4" t="s">
+        <v>24</v>
+      </c>
+      <c r="E4" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>46</v>
+      </c>
+      <c r="C5" t="s">
         <v>32</v>
       </c>
-      <c r="C2" t="s">
-        <v>24</v>
-      </c>
-      <c r="D2" t="s">
-        <v>27</v>
-      </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A3" t="s">
-        <v>23</v>
-      </c>
-      <c r="B3" t="s">
-        <v>25</v>
-      </c>
-      <c r="C3" t="s">
-        <v>28</v>
-      </c>
-      <c r="D3" t="s">
-        <v>29</v>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>47</v>
+      </c>
+      <c r="C6" t="s">
+        <v>33</v>
       </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="B4" t="s">
-        <v>33</v>
-      </c>
-      <c r="C4" t="s">
-        <v>26</v>
-      </c>
-      <c r="D4" t="s">
-        <v>31</v>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>48</v>
+      </c>
+      <c r="C7" t="s">
+        <v>34</v>
       </c>
     </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="B5" t="s">
-        <v>34</v>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>49</v>
+      </c>
+      <c r="C8" t="s">
+        <v>20</v>
       </c>
     </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="B6" t="s">
+    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>50</v>
+      </c>
+      <c r="C9" t="s">
         <v>35</v>
       </c>
     </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="B7" t="s">
+    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>51</v>
+      </c>
+      <c r="C10" t="s">
         <v>36</v>
       </c>
     </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="B8" t="s">
-        <v>22</v>
+    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
+        <v>52</v>
+      </c>
+      <c r="C11" t="s">
+        <v>37</v>
       </c>
     </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="B9" t="s">
-        <v>37</v>
+    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
+        <v>53</v>
+      </c>
+      <c r="C12" t="s">
+        <v>38</v>
       </c>
     </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="B10" t="s">
-        <v>38</v>
+    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
+        <v>54</v>
+      </c>
+      <c r="C13" t="s">
+        <v>39</v>
       </c>
     </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="B11" t="s">
-        <v>39</v>
+    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A14" t="s">
+        <v>55</v>
+      </c>
+      <c r="C14" t="s">
+        <v>40</v>
       </c>
     </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="B12" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="B13" t="s">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="B14" t="s">
-        <v>42</v>
+    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A15" t="s">
+        <v>56</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x010100F0286ABCF2CCF1469BE0D43457F463E3" ma:contentTypeVersion="16" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="615b81bd79b5a0f3eec299d039424273">
+  <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns3="ab62ed79-ca0d-44c9-85b3-522a3690b7b1" xmlns:ns4="490a895a-2a62-47fd-9986-d719414d7ad2" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="01de5d6703dbe4457944c9a4507e2b4e" ns3:_="" ns4:_="">
+    <xsd:import namespace="ab62ed79-ca0d-44c9-85b3-522a3690b7b1"/>
+    <xsd:import namespace="490a895a-2a62-47fd-9986-d719414d7ad2"/>
+    <xsd:element name="properties">
+      <xsd:complexType>
+        <xsd:sequence>
+          <xsd:element name="documentManagement">
+            <xsd:complexType>
+              <xsd:all>
+                <xsd:element ref="ns3:_activity" minOccurs="0"/>
+                <xsd:element ref="ns4:SharedWithUsers" minOccurs="0"/>
+                <xsd:element ref="ns4:SharedWithDetails" minOccurs="0"/>
+                <xsd:element ref="ns4:SharingHintHash" minOccurs="0"/>
+                <xsd:element ref="ns3:MediaServiceMetadata" minOccurs="0"/>
+                <xsd:element ref="ns3:MediaServiceFastMetadata" minOccurs="0"/>
+                <xsd:element ref="ns3:MediaServiceDateTaken" minOccurs="0"/>
+                <xsd:element ref="ns3:MediaServiceObjectDetectorVersions" minOccurs="0"/>
+                <xsd:element ref="ns3:MediaServiceAutoTags" minOccurs="0"/>
+                <xsd:element ref="ns3:MediaServiceGenerationTime" minOccurs="0"/>
+                <xsd:element ref="ns3:MediaServiceEventHashCode" minOccurs="0"/>
+                <xsd:element ref="ns3:MediaLengthInSeconds" minOccurs="0"/>
+                <xsd:element ref="ns3:MediaServiceSystemTags" minOccurs="0"/>
+                <xsd:element ref="ns3:MediaServiceLocation" minOccurs="0"/>
+                <xsd:element ref="ns3:MediaServiceOCR" minOccurs="0"/>
+                <xsd:element ref="ns3:MediaServiceSearchProperties" minOccurs="0"/>
+              </xsd:all>
+            </xsd:complexType>
+          </xsd:element>
+        </xsd:sequence>
+      </xsd:complexType>
+    </xsd:element>
+  </xsd:schema>
+  <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:dms="http://schemas.microsoft.com/office/2006/documentManagement/types" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls" targetNamespace="ab62ed79-ca0d-44c9-85b3-522a3690b7b1" elementFormDefault="qualified">
+    <xsd:import namespace="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <xsd:import namespace="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <xsd:element name="_activity" ma:index="8" nillable="true" ma:displayName="_activity" ma:hidden="true" ma:internalName="_activity">
+      <xsd:simpleType>
+        <xsd:restriction base="dms:Note"/>
+      </xsd:simpleType>
+    </xsd:element>
+    <xsd:element name="MediaServiceMetadata" ma:index="12" nillable="true" ma:displayName="MediaServiceMetadata" ma:hidden="true" ma:internalName="MediaServiceMetadata" ma:readOnly="true">
+      <xsd:simpleType>
+        <xsd:restriction base="dms:Note"/>
+      </xsd:simpleType>
+    </xsd:element>
+    <xsd:element name="MediaServiceFastMetadata" ma:index="13" nillable="true" ma:displayName="MediaServiceFastMetadata" ma:hidden="true" ma:internalName="MediaServiceFastMetadata" ma:readOnly="true">
+      <xsd:simpleType>
+        <xsd:restriction base="dms:Note"/>
+      </xsd:simpleType>
+    </xsd:element>
+    <xsd:element name="MediaServiceDateTaken" ma:index="14" nillable="true" ma:displayName="MediaServiceDateTaken" ma:hidden="true" ma:indexed="true" ma:internalName="MediaServiceDateTaken" ma:readOnly="true">
+      <xsd:simpleType>
+        <xsd:restriction base="dms:Text"/>
+      </xsd:simpleType>
+    </xsd:element>
+    <xsd:element name="MediaServiceObjectDetectorVersions" ma:index="15" nillable="true" ma:displayName="MediaServiceObjectDetectorVersions" ma:hidden="true" ma:indexed="true" ma:internalName="MediaServiceObjectDetectorVersions" ma:readOnly="true">
+      <xsd:simpleType>
+        <xsd:restriction base="dms:Text"/>
+      </xsd:simpleType>
+    </xsd:element>
+    <xsd:element name="MediaServiceAutoTags" ma:index="16" nillable="true" ma:displayName="Tags" ma:internalName="MediaServiceAutoTags" ma:readOnly="true">
+      <xsd:simpleType>
+        <xsd:restriction base="dms:Text"/>
+      </xsd:simpleType>
+    </xsd:element>
+    <xsd:element name="MediaServiceGenerationTime" ma:index="17" nillable="true" ma:displayName="MediaServiceGenerationTime" ma:hidden="true" ma:internalName="MediaServiceGenerationTime" ma:readOnly="true">
+      <xsd:simpleType>
+        <xsd:restriction base="dms:Text"/>
+      </xsd:simpleType>
+    </xsd:element>
+    <xsd:element name="MediaServiceEventHashCode" ma:index="18" nillable="true" ma:displayName="MediaServiceEventHashCode" ma:hidden="true" ma:internalName="MediaServiceEventHashCode" ma:readOnly="true">
+      <xsd:simpleType>
+        <xsd:restriction base="dms:Text"/>
+      </xsd:simpleType>
+    </xsd:element>
+    <xsd:element name="MediaLengthInSeconds" ma:index="19" nillable="true" ma:displayName="MediaLengthInSeconds" ma:hidden="true" ma:internalName="MediaLengthInSeconds" ma:readOnly="true">
+      <xsd:simpleType>
+        <xsd:restriction base="dms:Unknown"/>
+      </xsd:simpleType>
+    </xsd:element>
+    <xsd:element name="MediaServiceSystemTags" ma:index="20" nillable="true" ma:displayName="MediaServiceSystemTags" ma:hidden="true" ma:internalName="MediaServiceSystemTags" ma:readOnly="true">
+      <xsd:simpleType>
+        <xsd:restriction base="dms:Note"/>
+      </xsd:simpleType>
+    </xsd:element>
+    <xsd:element name="MediaServiceLocation" ma:index="21" nillable="true" ma:displayName="Location" ma:indexed="true" ma:internalName="MediaServiceLocation" ma:readOnly="true">
+      <xsd:simpleType>
+        <xsd:restriction base="dms:Text"/>
+      </xsd:simpleType>
+    </xsd:element>
+    <xsd:element name="MediaServiceOCR" ma:index="22" nillable="true" ma:displayName="Extracted Text" ma:internalName="MediaServiceOCR" ma:readOnly="true">
+      <xsd:simpleType>
+        <xsd:restriction base="dms:Note">
+          <xsd:maxLength value="255"/>
+        </xsd:restriction>
+      </xsd:simpleType>
+    </xsd:element>
+    <xsd:element name="MediaServiceSearchProperties" ma:index="23" nillable="true" ma:displayName="MediaServiceSearchProperties" ma:hidden="true" ma:internalName="MediaServiceSearchProperties" ma:readOnly="true">
+      <xsd:simpleType>
+        <xsd:restriction base="dms:Note"/>
+      </xsd:simpleType>
+    </xsd:element>
+  </xsd:schema>
+  <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:dms="http://schemas.microsoft.com/office/2006/documentManagement/types" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls" targetNamespace="490a895a-2a62-47fd-9986-d719414d7ad2" elementFormDefault="qualified">
+    <xsd:import namespace="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <xsd:import namespace="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <xsd:element name="SharedWithUsers" ma:index="9" nillable="true" ma:displayName="Shared With" ma:internalName="SharedWithUsers" ma:readOnly="true">
+      <xsd:complexType>
+        <xsd:complexContent>
+          <xsd:extension base="dms:UserMulti">
+            <xsd:sequence>
+              <xsd:element name="UserInfo" minOccurs="0" maxOccurs="unbounded">
+                <xsd:complexType>
+                  <xsd:sequence>
+                    <xsd:element name="DisplayName" type="xsd:string" minOccurs="0"/>
+                    <xsd:element name="AccountId" type="dms:UserId" minOccurs="0" nillable="true"/>
+                    <xsd:element name="AccountType" type="xsd:string" minOccurs="0"/>
+                  </xsd:sequence>
+                </xsd:complexType>
+              </xsd:element>
+            </xsd:sequence>
+          </xsd:extension>
+        </xsd:complexContent>
+      </xsd:complexType>
+    </xsd:element>
+    <xsd:element name="SharedWithDetails" ma:index="10" nillable="true" ma:displayName="Shared With Details" ma:internalName="SharedWithDetails" ma:readOnly="true">
+      <xsd:simpleType>
+        <xsd:restriction base="dms:Note">
+          <xsd:maxLength value="255"/>
+        </xsd:restriction>
+      </xsd:simpleType>
+    </xsd:element>
+    <xsd:element name="SharingHintHash" ma:index="11" nillable="true" ma:displayName="Sharing Hint Hash" ma:hidden="true" ma:internalName="SharingHintHash" ma:readOnly="true">
+      <xsd:simpleType>
+        <xsd:restriction base="dms:Text"/>
+      </xsd:simpleType>
+    </xsd:element>
+  </xsd:schema>
+  <xsd:schema xmlns="http://schemas.openxmlformats.org/package/2006/metadata/core-properties" xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:dc="http://purl.org/dc/elements/1.1/" xmlns:dcterms="http://purl.org/dc/terms/" xmlns:odoc="http://schemas.microsoft.com/internal/obd" targetNamespace="http://schemas.openxmlformats.org/package/2006/metadata/core-properties" elementFormDefault="qualified" attributeFormDefault="unqualified" blockDefault="#all">
+    <xsd:import namespace="http://purl.org/dc/elements/1.1/" schemaLocation="http://dublincore.org/schemas/xmls/qdc/2003/04/02/dc.xsd"/>
+    <xsd:import namespace="http://purl.org/dc/terms/" schemaLocation="http://dublincore.org/schemas/xmls/qdc/2003/04/02/dcterms.xsd"/>
+    <xsd:element name="coreProperties" type="CT_coreProperties"/>
+    <xsd:complexType name="CT_coreProperties">
+      <xsd:all>
+        <xsd:element ref="dc:creator" minOccurs="0" maxOccurs="1"/>
+        <xsd:element ref="dcterms:created" minOccurs="0" maxOccurs="1"/>
+        <xsd:element ref="dc:identifier" minOccurs="0" maxOccurs="1"/>
+        <xsd:element name="contentType" minOccurs="0" maxOccurs="1" type="xsd:string" ma:index="0" ma:displayName="Content Type"/>
+        <xsd:element ref="dc:title" minOccurs="0" maxOccurs="1" ma:index="4" ma:displayName="Title"/>
+        <xsd:element ref="dc:subject" minOccurs="0" maxOccurs="1"/>
+        <xsd:element ref="dc:description" minOccurs="0" maxOccurs="1"/>
+        <xsd:element name="keywords" minOccurs="0" maxOccurs="1" type="xsd:string"/>
+        <xsd:element ref="dc:language" minOccurs="0" maxOccurs="1"/>
+        <xsd:element name="category" minOccurs="0" maxOccurs="1" type="xsd:string"/>
+        <xsd:element name="version" minOccurs="0" maxOccurs="1" type="xsd:string"/>
+        <xsd:element name="revision" minOccurs="0" maxOccurs="1" type="xsd:string">
+          <xsd:annotation>
+            <xsd:documentation>
+                        This value indicates the number of saves or revisions. The application is responsible for updating this value after each revision.
+                    </xsd:documentation>
+          </xsd:annotation>
+        </xsd:element>
+        <xsd:element name="lastModifiedBy" minOccurs="0" maxOccurs="1" type="xsd:string"/>
+        <xsd:element ref="dcterms:modified" minOccurs="0" maxOccurs="1"/>
+        <xsd:element name="contentStatus" minOccurs="0" maxOccurs="1" type="xsd:string"/>
+      </xsd:all>
+    </xsd:complexType>
+  </xsd:schema>
+  <xs:schema xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls" xmlns:xs="http://www.w3.org/2001/XMLSchema" targetNamespace="http://schemas.microsoft.com/office/infopath/2007/PartnerControls" elementFormDefault="qualified" attributeFormDefault="unqualified">
+    <xs:element name="Person">
+      <xs:complexType>
+        <xs:sequence>
+          <xs:element ref="pc:DisplayName" minOccurs="0"/>
+          <xs:element ref="pc:AccountId" minOccurs="0"/>
+          <xs:element ref="pc:AccountType" minOccurs="0"/>
+        </xs:sequence>
+      </xs:complexType>
+    </xs:element>
+    <xs:element name="DisplayName" type="xs:string"/>
+    <xs:element name="AccountId" type="xs:string"/>
+    <xs:element name="AccountType" type="xs:string"/>
+    <xs:element name="BDCAssociatedEntity">
+      <xs:complexType>
+        <xs:sequence>
+          <xs:element ref="pc:BDCEntity" minOccurs="0" maxOccurs="unbounded"/>
+        </xs:sequence>
+        <xs:attribute ref="pc:EntityNamespace"/>
+        <xs:attribute ref="pc:EntityName"/>
+        <xs:attribute ref="pc:SystemInstanceName"/>
+        <xs:attribute ref="pc:AssociationName"/>
+      </xs:complexType>
+    </xs:element>
+    <xs:attribute name="EntityNamespace" type="xs:string"/>
+    <xs:attribute name="EntityName" type="xs:string"/>
+    <xs:attribute name="SystemInstanceName" type="xs:string"/>
+    <xs:attribute name="AssociationName" type="xs:string"/>
+    <xs:element name="BDCEntity">
+      <xs:complexType>
+        <xs:sequence>
+          <xs:element ref="pc:EntityDisplayName" minOccurs="0"/>
+          <xs:element ref="pc:EntityInstanceReference" minOccurs="0"/>
+          <xs:element ref="pc:EntityId1" minOccurs="0"/>
+          <xs:element ref="pc:EntityId2" minOccurs="0"/>
+          <xs:element ref="pc:EntityId3" minOccurs="0"/>
+          <xs:element ref="pc:EntityId4" minOccurs="0"/>
+          <xs:element ref="pc:EntityId5" minOccurs="0"/>
+        </xs:sequence>
+      </xs:complexType>
+    </xs:element>
+    <xs:element name="EntityDisplayName" type="xs:string"/>
+    <xs:element name="EntityInstanceReference" type="xs:string"/>
+    <xs:element name="EntityId1" type="xs:string"/>
+    <xs:element name="EntityId2" type="xs:string"/>
+    <xs:element name="EntityId3" type="xs:string"/>
+    <xs:element name="EntityId4" type="xs:string"/>
+    <xs:element name="EntityId5" type="xs:string"/>
+    <xs:element name="Terms">
+      <xs:complexType>
+        <xs:sequence>
+          <xs:element ref="pc:TermInfo" minOccurs="0" maxOccurs="unbounded"/>
+        </xs:sequence>
+      </xs:complexType>
+    </xs:element>
+    <xs:element name="TermInfo">
+      <xs:complexType>
+        <xs:sequence>
+          <xs:element ref="pc:TermName" minOccurs="0"/>
+          <xs:element ref="pc:TermId" minOccurs="0"/>
+        </xs:sequence>
+      </xs:complexType>
+    </xs:element>
+    <xs:element name="TermName" type="xs:string"/>
+    <xs:element name="TermId" type="xs:string"/>
+  </xs:schema>
+</ct:contentTypeSchema>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <_activity xmlns="ab62ed79-ca0d-44c9-85b3-522a3690b7b1" xsi:nil="true"/>
+  </documentManagement>
+</p:properties>
+</file>
+
+<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{4BE6E165-F187-407B-BABF-1CF38DA8FEAF}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{FF19AC07-0243-4A2B-BE93-63388EEFAB93}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/2001/XMLSchema"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="ab62ed79-ca0d-44c9-85b3-522a3690b7b1"/>
+    <ds:schemaRef ds:uri="490a895a-2a62-47fd-9986-d719414d7ad2"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{2A32DA2C-B8F9-4D6A-8249-948D4CF8672F}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="490a895a-2a62-47fd-9986-d719414d7ad2"/>
+    <ds:schemaRef ds:uri="ab62ed79-ca0d-44c9-85b3-522a3690b7b1"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
Update copy on table calculator page, add context hint to fvn cell in excel spreadsheet
</commit_message>
<xml_diff>
--- a/www/example-NPM-data.xlsx
+++ b/www/example-NPM-data.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\maeve\Documents\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\wsl.localhost\Ubuntu-24.04\home\maeve\cdrc\edits-NPM-Calculator\www\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{E63A4015-A377-4DAC-B30C-D526C7ED5D35}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{49E824AB-2A40-42D0-ABAD-23C7A239AC7B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -734,10 +734,6 @@
     </ext>
   </extLst>
 </styleSheet>
-</file>
-
-<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
-<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -1040,7 +1036,7 @@
   <dimension ref="A1:U1"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="H1" workbookViewId="0">
-      <selection activeCell="S2" sqref="S2"/>
+      <selection activeCell="G3" sqref="G3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1132,6 +1128,12 @@
       </c>
     </row>
   </sheetData>
+  <dataValidations count="1">
+    <dataValidation type="decimal" showInputMessage="1" showErrorMessage="1" promptTitle="Do not leave blank" prompt="Enter 0 if there is no fvn content" sqref="R2:R1048576" xr:uid="{95D17293-1294-4818-A7D4-AE8BF197D555}">
+      <formula1>0</formula1>
+      <formula2>100</formula2>
+    </dataValidation>
+  </dataValidations>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="0" copies="0" r:id="rId1"/>
   <extLst>
@@ -1345,12 +1347,11 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <_activity xmlns="ab62ed79-ca0d-44c9-85b3-522a3690b7b1" xsi:nil="true"/>
+  </documentManagement>
+</p:properties>
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
@@ -1593,17 +1594,27 @@
 </file>
 
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <_activity xmlns="ab62ed79-ca0d-44c9-85b3-522a3690b7b1" xsi:nil="true"/>
-  </documentManagement>
-</p:properties>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{4BE6E165-F187-407B-BABF-1CF38DA8FEAF}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{2A32DA2C-B8F9-4D6A-8249-948D4CF8672F}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="490a895a-2a62-47fd-9986-d719414d7ad2"/>
+    <ds:schemaRef ds:uri="ab62ed79-ca0d-44c9-85b3-522a3690b7b1"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
@@ -1628,18 +1639,9 @@
 </file>
 
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{2A32DA2C-B8F9-4D6A-8249-948D4CF8672F}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{4BE6E165-F187-407B-BABF-1CF38DA8FEAF}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="490a895a-2a62-47fd-9986-d719414d7ad2"/>
-    <ds:schemaRef ds:uri="ab62ed79-ca0d-44c9-85b3-522a3690b7b1"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
</xml_diff>